<commit_message>
Add script tools to build instructions
</commit_message>
<xml_diff>
--- a/doc/FayLang.xlsx
+++ b/doc/FayLang.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27885" yWindow="0" windowWidth="12660" windowHeight="8160" activeTab="1"/>
+    <workbookView xWindow="30030" yWindow="0" windowWidth="12660" windowHeight="8160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Math" sheetId="1" r:id="rId1"/>
-    <sheet name="Instruct" sheetId="4" r:id="rId2"/>
+    <sheet name="Inst" sheetId="4" r:id="rId2"/>
     <sheet name="ASTType" sheetId="5" r:id="rId3"/>
     <sheet name="PSTType" sheetId="6" r:id="rId4"/>
     <sheet name="TokenType" sheetId="7" r:id="rId5"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="309">
   <si>
     <t>[ ]</t>
   </si>
@@ -511,14 +511,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>P4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Text</t>
   </si>
   <si>
@@ -707,58 +699,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Active</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Comment</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>字节值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>整形</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Length</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>长整型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>浮点数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>双精度浮点数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>布尔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符串</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对象</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>函数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PopTo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -771,15 +719,405 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>byte</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>long</t>
+    <t>Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FixedValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Expr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Call</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Params</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Void</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Semicolon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comma</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LeftBrace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RightBrace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>操作符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DoubleSlash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注释</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Using</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Var</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DescSymbol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SystemName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Else</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElseIf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Foreach</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>While</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Return</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BasicType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Char</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Call</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Static</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Disabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>typeIndex:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>funIndex:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>函数</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>没有值类型</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>字节值</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>整形</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>长整型</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>浮点数</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>双精度浮点数</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>布尔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>字符串</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>对象</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int32_t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unsigned char</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int64_t</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -795,147 +1133,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Comment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Empty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FixedValue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Expr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Call</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Assign</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Params</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>参数列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Void</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>没有值类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>None</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Assign</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Colon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Comment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>=</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Semicolon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Comma</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LeftBrace</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RightBrace</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>操作符</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DoubleSlash</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>//</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>注释</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Using</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Package</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Var</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Class</t>
+    <t>std::string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>void*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Virtual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用静态方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用普通方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用虚方法</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -943,67 +1161,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DescSymbol</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SystemName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Else</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ElseIf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>For</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Foreach</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>While</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Return</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BasicType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Char</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fun</t>
+    <t>Special</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用接口的方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>val:byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>val:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>val:long</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>val:float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>val:double</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>val:bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>val:string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>count:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paramCount:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>outsideFunIndex:int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1011,7 +1213,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1049,14 +1251,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="7" tint="0.59999389629810485"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
       <family val="2"/>
@@ -1079,8 +1273,41 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="DejaVu Sans Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="DejaVu Sans YuanTi Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="DejaVu Sans Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="DejaVu Sans YuanTi Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1089,17 +1316,62 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1108,7 +1380,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1121,23 +1393,77 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1541,43 +1867,43 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="5">
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="5">
+    <row r="7" spans="1:8" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="4">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2361,401 +2687,467 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" style="8"/>
-    <col min="2" max="3" width="16.625" style="3" customWidth="1"/>
-    <col min="4" max="8" width="11.25" style="3" customWidth="1"/>
-    <col min="9" max="9" width="34.125" style="3" customWidth="1"/>
-    <col min="10" max="11" width="11.25" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="4" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10.125" style="12" customWidth="1"/>
+    <col min="4" max="5" width="10.125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="21.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.375" style="16" customWidth="1"/>
+    <col min="9" max="11" width="16.75" style="18" customWidth="1"/>
+    <col min="12" max="12" width="57.875" style="17" customWidth="1"/>
+    <col min="13" max="14" width="11.25" style="9" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="13">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C3" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" s="13">
+        <v>2</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C4" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" s="13">
+        <v>3</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C5" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" s="13">
+        <v>4</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C6" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D6" s="13">
+        <v>5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C7" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D7" s="13">
+        <v>6</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C8" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="13">
+        <v>7</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="11">
+        <v>2</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="11">
+        <v>3</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="F10" s="16" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="11">
+        <v>4</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C12" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E12" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C13" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C14" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="E14" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C15" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="E15" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C16" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="E16" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B6" s="3" t="s">
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C17" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="E17" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B18" s="11">
+        <v>5</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="E18" s="14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C19" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C20" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C21" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C22" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C23" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C24" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B25" s="11">
+        <v>6</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C26" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C27" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C28" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C29" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
+      <c r="E29" s="14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C30" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="E30" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C31" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="E31" s="14" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>198</v>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B32" s="11">
+        <v>7</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D32" s="13">
+        <v>1</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="J32" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="L32" s="27" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C33" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D33" s="13">
+        <v>2</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="J33" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="L33" s="27" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C34" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D34" s="13">
+        <v>3</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="I34" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="J34" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="L34" s="27" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C35" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D35" s="13">
+        <v>4</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="J35" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="L35" s="27" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -2770,7 +3162,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -2780,148 +3172,148 @@
     <col min="3" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>172</v>
+    <row r="1" spans="1:2" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2946,70 +3338,70 @@
     <col min="3" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>229</v>
+    <row r="1" spans="1:2" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3033,194 +3425,194 @@
     <col min="2" max="2" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>244</v>
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="B4" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="B5" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="B6" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="B7" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="B8" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="B9" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="B10" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B11" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -3232,138 +3624,204 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="16.25" style="7" customWidth="1"/>
-    <col min="3" max="3" width="27.5" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="3"/>
+    <col min="1" max="4" width="16.25" style="8" customWidth="1"/>
+    <col min="5" max="5" width="27.5" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" s="26" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="B2" s="7">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="B4" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8">
+        <v>4</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B5" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="C5" s="8">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C6" s="8">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C7" s="8">
+        <v>6</v>
+      </c>
+      <c r="D7" s="8">
+        <v>8</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="C8" s="8">
+        <v>7</v>
+      </c>
+      <c r="D8" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="B4" s="7">
-        <v>4</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B5" s="7">
+      <c r="E8" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="C9" s="8">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="B6" s="7">
-        <v>4</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="B7" s="7">
+      <c r="D9" s="8">
         <v>8</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="E9" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="B8" s="7">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="B10" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C10" s="8">
+        <v>9</v>
+      </c>
+      <c r="D10" s="8">
+        <v>8</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B11" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" s="8">
+        <v>10</v>
+      </c>
+      <c r="D11" s="8">
         <v>8</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="B10" s="7">
-        <v>8</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B11" s="7">
-        <v>8</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>218</v>
+      <c r="E11" s="8" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move instruction code to excel file
</commit_message>
<xml_diff>
--- a/doc/FayLang.xlsx
+++ b/doc/FayLang.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30030" yWindow="0" windowWidth="12660" windowHeight="8160" activeTab="1"/>
+    <workbookView xWindow="2145" yWindow="0" windowWidth="12660" windowHeight="8160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Math" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="TokenType" sheetId="7" r:id="rId4"/>
     <sheet name="ValueType" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="304">
   <si>
     <t>[ ]</t>
   </si>
@@ -1183,6 +1183,27 @@
       </rPr>
       <t>注释</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stack.push(new FayValue(#p1));</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PTR(FayFun) fun=this-&gt;_domain-&gt;findFun(#v1,#v2);
+this-&gt;run(fun);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete stack.pop();</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1282,7 +1303,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1291,13 +1312,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1315,13 +1330,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1336,16 +1351,16 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="0"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="0"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="0"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1355,7 +1370,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1380,62 +1395,53 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2659,466 +2665,638 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="11" customWidth="1"/>
-    <col min="4" max="5" width="10.125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="21.625" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.125" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.375" style="15" customWidth="1"/>
-    <col min="9" max="11" width="16.75" style="17" customWidth="1"/>
-    <col min="12" max="12" width="57.875" style="16" customWidth="1"/>
-    <col min="13" max="14" width="11.25" style="8" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="8"/>
+    <col min="1" max="1" width="15" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" style="16" customWidth="1"/>
+    <col min="3" max="6" width="10.125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="21.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.375" style="13" customWidth="1"/>
+    <col min="10" max="12" width="16.75" style="14" customWidth="1"/>
+    <col min="13" max="13" width="59" style="19" customWidth="1"/>
+    <col min="14" max="14" width="57.875" style="20" customWidth="1"/>
+    <col min="15" max="16" width="11.25" style="12" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="J1" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="K1" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="L1" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="N1" s="18" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="10">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="str">
+        <f>D2&amp;F2</f>
+        <v>PushByte</v>
+      </c>
+      <c r="C2" s="16">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="D2" s="12">
+      <c r="E2" s="16">
         <v>1</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C3" s="11" t="s">
+      <c r="M2" s="19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="str">
+        <f t="shared" ref="A3:A35" si="0">D3&amp;F3</f>
+        <v>PushInt</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="D3" s="12">
+      <c r="E3" s="16">
         <v>2</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C4" s="11" t="s">
+      <c r="M3" s="19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>PushLong</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="D4" s="12">
+      <c r="E4" s="16">
         <v>3</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C5" s="11" t="s">
+      <c r="M4" s="19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>PushFloat</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="D5" s="12">
+      <c r="E5" s="16">
         <v>4</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C6" s="11" t="s">
+      <c r="M5" s="19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>PushDouble</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="D6" s="12">
+      <c r="E6" s="16">
         <v>5</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C7" s="11" t="s">
+      <c r="M6" s="19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>PushBool</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="D7" s="12">
+      <c r="E7" s="16">
         <v>6</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C8" s="11" t="s">
+      <c r="M7" s="19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>PushString</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="D8" s="12">
+      <c r="E8" s="16">
         <v>7</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="10">
+      <c r="M8" s="19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>Pop</v>
+      </c>
+      <c r="C9" s="16">
         <v>2</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="16" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="10">
+      <c r="M9" s="19" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>PopTo</v>
+      </c>
+      <c r="C10" s="16">
         <v>3</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D10" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="G10" s="13" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="10">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>IntToByte</v>
+      </c>
+      <c r="C11" s="16">
         <v>4</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="F11" s="16" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C12" s="11" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>IntToInt</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="F12" s="16" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C13" s="11" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>IntToLong</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="F13" s="16" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C14" s="11" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>IntToFloat</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="F14" s="16" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C15" s="11" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>IntToDouble</v>
+      </c>
+      <c r="D15" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="F15" s="16" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C16" s="11" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>IntToBool</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="F16" s="16" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C17" s="11" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>IntToString</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="F17" s="16" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="10">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>AddByte</v>
+      </c>
+      <c r="C18" s="16">
         <v>5</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="F18" s="16" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C19" s="11" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>AddInt</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="F19" s="16" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C20" s="11" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>AddLong</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="F20" s="16" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C21" s="11" t="s">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>AddFloat</v>
+      </c>
+      <c r="D21" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="F21" s="16" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C22" s="11" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>AddDouble</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="F22" s="16" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C23" s="11" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>AddBool</v>
+      </c>
+      <c r="D23" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="F23" s="16" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C24" s="11" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>AddString</v>
+      </c>
+      <c r="D24" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="F24" s="16" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="10">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>SubByte</v>
+      </c>
+      <c r="C25" s="16">
         <v>6</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="D25" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="F25" s="16" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C26" s="11" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>SubInt</v>
+      </c>
+      <c r="D26" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="F26" s="16" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C27" s="11" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>SubLong</v>
+      </c>
+      <c r="D27" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="F27" s="16" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C28" s="11" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>SubFloat</v>
+      </c>
+      <c r="D28" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="F28" s="16" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C29" s="11" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>SubDouble</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="F29" s="16" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C30" s="11" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>SubBool</v>
+      </c>
+      <c r="D30" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="F30" s="16" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C31" s="11" t="s">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>SubString</v>
+      </c>
+      <c r="D31" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="F31" s="16" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B32" s="10">
+    <row r="32" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>CallStatic</v>
+      </c>
+      <c r="C32" s="16">
         <v>7</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="D32" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="D32" s="12">
+      <c r="E32" s="16">
         <v>1</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="F32" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="G32" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="G32" s="15" t="s">
+      <c r="H32" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I32" s="17" t="s">
+      <c r="J32" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="J32" s="17" t="s">
+      <c r="K32" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="L32" s="26" t="s">
+      <c r="M32" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="N32" s="21" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C33" s="11" t="s">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>CallSpecial</v>
+      </c>
+      <c r="D33" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="D33" s="12">
+      <c r="E33" s="16">
         <v>2</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="F33" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="G33" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="G33" s="15" t="s">
+      <c r="H33" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I33" s="17" t="s">
+      <c r="J33" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="J33" s="17" t="s">
+      <c r="K33" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="L33" s="26" t="s">
+      <c r="N33" s="21" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C34" s="11" t="s">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>CallVirtual</v>
+      </c>
+      <c r="D34" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="D34" s="12">
+      <c r="E34" s="16">
         <v>3</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="F34" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="G34" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="H34" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I34" s="17" t="s">
+      <c r="J34" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="J34" s="17" t="s">
+      <c r="K34" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="L34" s="26" t="s">
+      <c r="N34" s="21" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C35" s="11" t="s">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>CallInterface</v>
+      </c>
+      <c r="D35" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="D35" s="12">
+      <c r="E35" s="16">
         <v>4</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="F35" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="F35" s="15" t="s">
+      <c r="G35" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="G35" s="15" t="s">
+      <c r="H35" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I35" s="17" t="s">
+      <c r="J35" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="J35" s="17" t="s">
+      <c r="K35" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="L35" s="26" t="s">
+      <c r="N35" s="21" t="s">
         <v>286</v>
       </c>
     </row>
@@ -3310,11 +3488,11 @@
     <col min="3" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="8" t="s">
         <v>214</v>
       </c>
     </row>
@@ -3522,20 +3700,20 @@
     <col min="6" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="8" t="s">
         <v>204</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change name and order
</commit_message>
<xml_diff>
--- a/doc/FayLang.xlsx
+++ b/doc/FayLang.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="310">
   <si>
     <t>[ ]</t>
   </si>
@@ -1092,6 +1092,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Fun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Virtual</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1109,10 +1113,6 @@
   </si>
   <si>
     <t>Interface</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Special</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1204,6 +1204,30 @@
   </si>
   <si>
     <t>delete stack.pop();</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Long</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Double</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2668,10 +2692,10 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2736,7 +2760,7 @@
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="str">
         <f>D2&amp;F2</f>
-        <v>PushByte</v>
+        <v>PushBool</v>
       </c>
       <c r="C2" s="16">
         <v>1</v>
@@ -2745,13 +2769,13 @@
         <v>199</v>
       </c>
       <c r="E2" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>190</v>
+        <v>304</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="M2" s="19" t="s">
         <v>301</v>
@@ -2760,19 +2784,19 @@
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="str">
         <f t="shared" ref="A3:A35" si="0">D3&amp;F3</f>
-        <v>PushInt</v>
+        <v>PushByte</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>199</v>
       </c>
       <c r="E3" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>191</v>
+        <v>305</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M3" s="19" t="s">
         <v>301</v>
@@ -2781,19 +2805,19 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>PushLong</v>
+        <v>PushInt</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>199</v>
       </c>
       <c r="E4" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>192</v>
+        <v>306</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M4" s="19" t="s">
         <v>301</v>
@@ -2802,19 +2826,19 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>PushFloat</v>
+        <v>PushLong</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>199</v>
       </c>
       <c r="E5" s="16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>193</v>
+        <v>308</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M5" s="19" t="s">
         <v>301</v>
@@ -2823,19 +2847,19 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>PushDouble</v>
+        <v>PushFloat</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>199</v>
       </c>
       <c r="E6" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>194</v>
+        <v>307</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="M6" s="19" t="s">
         <v>301</v>
@@ -2844,19 +2868,19 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>PushBool</v>
+        <v>PushDouble</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>199</v>
       </c>
       <c r="E7" s="16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>195</v>
+        <v>309</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M7" s="19" t="s">
         <v>301</v>
@@ -2871,7 +2895,7 @@
         <v>199</v>
       </c>
       <c r="E8" s="16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>196</v>
@@ -3207,13 +3231,13 @@
         <v>302</v>
       </c>
       <c r="N32" s="21" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>CallSpecial</v>
+        <v>CallFun</v>
       </c>
       <c r="D33" s="16" t="s">
         <v>252</v>
@@ -3222,7 +3246,7 @@
         <v>2</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>296</v>
@@ -3237,7 +3261,7 @@
         <v>258</v>
       </c>
       <c r="N33" s="21" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -3252,7 +3276,7 @@
         <v>3</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G34" s="13" t="s">
         <v>296</v>
@@ -3267,7 +3291,7 @@
         <v>258</v>
       </c>
       <c r="N34" s="21" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
@@ -3282,7 +3306,7 @@
         <v>4</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>296</v>
@@ -3690,7 +3714,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3736,10 +3760,10 @@
     </row>
     <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C3" s="7">
         <v>2</v>
@@ -3748,92 +3772,92 @@
         <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C4" s="7">
         <v>3</v>
       </c>
       <c r="D4" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C5" s="7">
         <v>4</v>
       </c>
       <c r="D5" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C6" s="7">
         <v>5</v>
       </c>
       <c r="D6" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C7" s="7">
         <v>6</v>
       </c>
       <c r="D7" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C8" s="7">
         <v>7</v>
       </c>
       <c r="D8" s="7">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Improve fay language structure
</commit_message>
<xml_diff>
--- a/doc/FayLang.xlsx
+++ b/doc/FayLang.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\fay\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\fay\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
     <sheet name="TokenType" sheetId="7" r:id="rId4"/>
     <sheet name="ValueType" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="306">
   <si>
     <t>[ ]</t>
   </si>
@@ -1092,10 +1092,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Fun</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Virtual</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1104,19 +1100,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>调用普通方法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>调用虚方法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interface</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>调用接口的方法</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1198,44 +1182,44 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PTR(FayFun) fun=this-&gt;_domain-&gt;findFun(#v1,#v2);
+    <t>delete stack.pop();</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Long</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Double</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PTR(FayFun) fun=this-&gt;_domain-&gt;findFun(#v1,#v2,true);
 this-&gt;run(fun);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete stack.pop();</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Byte</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Float</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Long</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Double</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1753,7 +1737,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.125" style="1" customWidth="1"/>
@@ -1766,7 +1750,7 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>147</v>
       </c>
@@ -1789,7 +1773,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="18" customHeight="1">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -1809,7 +1793,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="18" customHeight="1">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1829,7 +1813,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="18" customHeight="1">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -1849,7 +1833,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -1869,7 +1853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="18" customHeight="1">
       <c r="B6" s="4">
         <v>2</v>
       </c>
@@ -1889,7 +1873,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" s="4" customFormat="1" ht="18" customHeight="1">
       <c r="B7" s="4">
         <v>2</v>
       </c>
@@ -1909,7 +1893,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B8" s="2">
         <v>2</v>
       </c>
@@ -1929,7 +1913,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B9" s="2">
         <v>2</v>
       </c>
@@ -1949,7 +1933,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="18" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>148</v>
       </c>
@@ -1972,7 +1956,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="18" customHeight="1">
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -1992,7 +1976,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B12" s="2">
         <v>2</v>
       </c>
@@ -2012,7 +1996,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="18" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>149</v>
       </c>
@@ -2035,7 +2019,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="18" customHeight="1">
       <c r="B14" s="1">
         <v>3</v>
       </c>
@@ -2055,7 +2039,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="18" customHeight="1">
       <c r="B15" s="1">
         <v>3</v>
       </c>
@@ -2075,7 +2059,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="18" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>140</v>
       </c>
@@ -2098,7 +2082,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="18" customHeight="1">
       <c r="B17" s="1">
         <v>4</v>
       </c>
@@ -2118,7 +2102,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="18" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>141</v>
       </c>
@@ -2144,7 +2128,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="18" customHeight="1">
       <c r="B19" s="1">
         <v>5</v>
       </c>
@@ -2167,7 +2151,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="18" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>142</v>
       </c>
@@ -2190,7 +2174,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="18" customHeight="1">
       <c r="B21" s="1">
         <v>6</v>
       </c>
@@ -2213,7 +2197,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="18" customHeight="1">
       <c r="B22" s="1">
         <v>6</v>
       </c>
@@ -2233,7 +2217,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="18" customHeight="1">
       <c r="B23" s="1">
         <v>6</v>
       </c>
@@ -2256,7 +2240,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="18" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>143</v>
       </c>
@@ -2282,7 +2266,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="18" customHeight="1">
       <c r="B25" s="1">
         <v>7</v>
       </c>
@@ -2305,7 +2289,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="18" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>144</v>
       </c>
@@ -2328,7 +2312,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="18" customHeight="1">
       <c r="B27" s="1">
         <v>9</v>
       </c>
@@ -2348,7 +2332,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="18" customHeight="1">
       <c r="B28" s="1">
         <v>10</v>
       </c>
@@ -2368,7 +2352,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="18" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>145</v>
       </c>
@@ -2394,7 +2378,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="18" customHeight="1">
       <c r="B30" s="1">
         <v>12</v>
       </c>
@@ -2417,7 +2401,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B31" s="2">
         <v>13</v>
       </c>
@@ -2437,7 +2421,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="18" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>146</v>
       </c>
@@ -2460,7 +2444,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B33" s="2">
         <v>14</v>
       </c>
@@ -2480,7 +2464,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B34" s="2">
         <v>14</v>
       </c>
@@ -2500,7 +2484,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B35" s="2">
         <v>14</v>
       </c>
@@ -2520,7 +2504,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B36" s="2">
         <v>14</v>
       </c>
@@ -2540,7 +2524,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B37" s="2">
         <v>14</v>
       </c>
@@ -2560,7 +2544,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B38" s="2">
         <v>14</v>
       </c>
@@ -2580,7 +2564,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B39" s="2">
         <v>14</v>
       </c>
@@ -2600,7 +2584,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B40" s="2">
         <v>14</v>
       </c>
@@ -2620,7 +2604,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B41" s="2">
         <v>14</v>
       </c>
@@ -2640,7 +2624,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B42" s="2">
         <v>14</v>
       </c>
@@ -2660,7 +2644,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="B43" s="2">
         <v>15</v>
       </c>
@@ -2689,16 +2673,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="15" style="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" style="16" customWidth="1"/>
@@ -2713,9 +2697,9 @@
     <col min="17" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="15.75">
       <c r="A1" s="22" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>256</v>
@@ -2751,13 +2735,13 @@
         <v>251</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="N1" s="18" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="23" t="str">
         <f>D2&amp;F2</f>
         <v>PushBool</v>
@@ -2772,18 +2756,18 @@
         <v>2</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="23" t="str">
-        <f t="shared" ref="A3:A35" si="0">D3&amp;F3</f>
+        <f t="shared" ref="A3:A33" si="0">D3&amp;F3</f>
         <v>PushByte</v>
       </c>
       <c r="D3" s="16" t="s">
@@ -2793,16 +2777,16 @@
         <v>3</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="M3" s="19" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="23" t="str">
         <f t="shared" si="0"/>
         <v>PushInt</v>
@@ -2814,16 +2798,16 @@
         <v>4</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="M4" s="19" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="23" t="str">
         <f t="shared" si="0"/>
         <v>PushLong</v>
@@ -2835,16 +2819,16 @@
         <v>5</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="M5" s="19" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>PushFloat</v>
@@ -2856,16 +2840,16 @@
         <v>6</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="M6" s="19" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="23" t="str">
         <f t="shared" si="0"/>
         <v>PushDouble</v>
@@ -2877,16 +2861,16 @@
         <v>7</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="23" t="str">
         <f t="shared" si="0"/>
         <v>PushString</v>
@@ -2901,13 +2885,13 @@
         <v>196</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="M8" s="19" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="23" t="str">
         <f t="shared" si="0"/>
         <v>Pop</v>
@@ -2919,10 +2903,10 @@
         <v>200</v>
       </c>
       <c r="M9" s="19" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="23" t="str">
         <f t="shared" si="0"/>
         <v>PopTo</v>
@@ -2934,10 +2918,10 @@
         <v>206</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="23" t="str">
         <f t="shared" si="0"/>
         <v>IntToByte</v>
@@ -2952,7 +2936,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" s="23" t="str">
         <f t="shared" si="0"/>
         <v>IntToInt</v>
@@ -2964,7 +2948,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" s="23" t="str">
         <f t="shared" si="0"/>
         <v>IntToLong</v>
@@ -2976,7 +2960,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" s="23" t="str">
         <f t="shared" si="0"/>
         <v>IntToFloat</v>
@@ -2988,7 +2972,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="A15" s="23" t="str">
         <f t="shared" si="0"/>
         <v>IntToDouble</v>
@@ -3000,7 +2984,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" s="23" t="str">
         <f t="shared" si="0"/>
         <v>IntToBool</v>
@@ -3012,7 +2996,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14">
       <c r="A17" s="23" t="str">
         <f t="shared" si="0"/>
         <v>IntToString</v>
@@ -3024,7 +3008,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14">
       <c r="A18" s="23" t="str">
         <f t="shared" si="0"/>
         <v>AddByte</v>
@@ -3039,7 +3023,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14">
       <c r="A19" s="23" t="str">
         <f t="shared" si="0"/>
         <v>AddInt</v>
@@ -3051,7 +3035,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14">
       <c r="A20" s="23" t="str">
         <f t="shared" si="0"/>
         <v>AddLong</v>
@@ -3063,7 +3047,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14">
       <c r="A21" s="23" t="str">
         <f t="shared" si="0"/>
         <v>AddFloat</v>
@@ -3075,7 +3059,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14">
       <c r="A22" s="23" t="str">
         <f t="shared" si="0"/>
         <v>AddDouble</v>
@@ -3087,7 +3071,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14">
       <c r="A23" s="23" t="str">
         <f t="shared" si="0"/>
         <v>AddBool</v>
@@ -3099,7 +3083,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14">
       <c r="A24" s="23" t="str">
         <f t="shared" si="0"/>
         <v>AddString</v>
@@ -3111,7 +3095,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14">
       <c r="A25" s="23" t="str">
         <f t="shared" si="0"/>
         <v>SubByte</v>
@@ -3126,7 +3110,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14">
       <c r="A26" s="23" t="str">
         <f t="shared" si="0"/>
         <v>SubInt</v>
@@ -3138,7 +3122,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14">
       <c r="A27" s="23" t="str">
         <f t="shared" si="0"/>
         <v>SubLong</v>
@@ -3150,7 +3134,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14">
       <c r="A28" s="23" t="str">
         <f t="shared" si="0"/>
         <v>SubFloat</v>
@@ -3162,7 +3146,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14">
       <c r="A29" s="23" t="str">
         <f t="shared" si="0"/>
         <v>SubDouble</v>
@@ -3174,7 +3158,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14">
       <c r="A30" s="23" t="str">
         <f t="shared" si="0"/>
         <v>SubBool</v>
@@ -3186,7 +3170,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14">
       <c r="A31" s="23" t="str">
         <f t="shared" si="0"/>
         <v>SubString</v>
@@ -3198,9 +3182,9 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="25.5">
       <c r="A32" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f>D32&amp;F32</f>
         <v>CallStatic</v>
       </c>
       <c r="C32" s="16">
@@ -3216,10 +3200,10 @@
         <v>253</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="J32" s="14" t="s">
         <v>257</v>
@@ -3228,31 +3212,31 @@
         <v>258</v>
       </c>
       <c r="M32" s="19" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="N32" s="21" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>CallFun</v>
+        <v>CallVirtual</v>
       </c>
       <c r="D33" s="16" t="s">
         <v>252</v>
       </c>
       <c r="E33" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>280</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="J33" s="14" t="s">
         <v>257</v>
@@ -3261,67 +3245,7 @@
         <v>258</v>
       </c>
       <c r="N33" s="21" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v>CallVirtual</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="E34" s="16">
-        <v>3</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>281</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="J34" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="K34" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="N34" s="21" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v>CallInterface</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="E35" s="16">
-        <v>4</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="J35" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="K35" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="N35" s="21" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3339,14 +3263,14 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="15.875" style="3" customWidth="1"/>
     <col min="2" max="2" width="35" style="3" customWidth="1"/>
     <col min="3" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="5" customFormat="1" ht="15">
       <c r="A1" s="5" t="s">
         <v>169</v>
       </c>
@@ -3354,7 +3278,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>153</v>
       </c>
@@ -3362,7 +3286,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
         <v>154</v>
       </c>
@@ -3370,7 +3294,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>207</v>
       </c>
@@ -3378,7 +3302,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>155</v>
       </c>
@@ -3386,7 +3310,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
         <v>156</v>
       </c>
@@ -3394,7 +3318,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
         <v>157</v>
       </c>
@@ -3402,7 +3326,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
         <v>158</v>
       </c>
@@ -3410,7 +3334,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
         <v>159</v>
       </c>
@@ -3418,7 +3342,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
         <v>160</v>
       </c>
@@ -3426,7 +3350,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
         <v>161</v>
       </c>
@@ -3434,7 +3358,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
         <v>162</v>
       </c>
@@ -3442,7 +3366,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
         <v>163</v>
       </c>
@@ -3450,7 +3374,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
         <v>164</v>
       </c>
@@ -3458,7 +3382,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
         <v>165</v>
       </c>
@@ -3466,7 +3390,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
         <v>166</v>
       </c>
@@ -3474,7 +3398,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
         <v>167</v>
       </c>
@@ -3482,7 +3406,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
         <v>168</v>
       </c>
@@ -3505,14 +3429,14 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="22.5" style="6" customWidth="1"/>
     <col min="2" max="2" width="39.375" style="6" customWidth="1"/>
     <col min="3" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>210</v>
       </c>
@@ -3520,12 +3444,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>212</v>
       </c>
@@ -3533,7 +3457,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>213</v>
       </c>
@@ -3541,7 +3465,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>217</v>
       </c>
@@ -3549,7 +3473,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>219</v>
       </c>
@@ -3557,7 +3481,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>221</v>
       </c>
@@ -3565,7 +3489,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>223</v>
       </c>
@@ -3573,15 +3497,15 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>225</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>226</v>
       </c>
@@ -3589,115 +3513,115 @@
         <v>227</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>214</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="15" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="15" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="15" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="15" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="15" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="15" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" ht="15" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" ht="15" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" ht="15" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" ht="15" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" ht="15" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" ht="15" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" ht="15" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" ht="15" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" ht="15" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" ht="15" customHeight="1">
       <c r="A28" s="6" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" ht="15" customHeight="1">
       <c r="A29" s="6" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" ht="15" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" ht="15" customHeight="1">
       <c r="A31" s="6" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" ht="15" customHeight="1">
       <c r="A32" s="6" t="s">
         <v>247</v>
       </c>
@@ -3717,14 +3641,14 @@
       <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="4" width="16.25" style="7" customWidth="1"/>
     <col min="5" max="5" width="27.5" style="7" customWidth="1"/>
     <col min="6" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="15.75">
       <c r="A1" s="8" t="s">
         <v>189</v>
       </c>
@@ -3741,7 +3665,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="16.5">
       <c r="A2" s="7" t="s">
         <v>209</v>
       </c>
@@ -3758,7 +3682,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="16.5">
       <c r="A3" s="7" t="s">
         <v>195</v>
       </c>
@@ -3775,7 +3699,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16.5">
       <c r="A4" s="7" t="s">
         <v>190</v>
       </c>
@@ -3792,7 +3716,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="16.5">
       <c r="A5" s="7" t="s">
         <v>191</v>
       </c>
@@ -3809,7 +3733,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="16.5">
       <c r="A6" s="7" t="s">
         <v>192</v>
       </c>
@@ -3826,7 +3750,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="16.5">
       <c r="A7" s="7" t="s">
         <v>193</v>
       </c>
@@ -3843,7 +3767,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="16.5">
       <c r="A8" s="7" t="s">
         <v>194</v>
       </c>
@@ -3860,7 +3784,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="16.5">
       <c r="A9" s="7" t="s">
         <v>196</v>
       </c>
@@ -3877,7 +3801,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="16.5">
       <c r="A10" s="7" t="s">
         <v>197</v>
       </c>
@@ -3894,7 +3818,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="16.5">
       <c r="A11" s="7" t="s">
         <v>198</v>
       </c>
@@ -3914,5 +3838,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change instruction maker flow from if to switch
</commit_message>
<xml_diff>
--- a/doc/FayLang.xlsx
+++ b/doc/FayLang.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="498">
   <si>
     <t>[ ]</t>
   </si>
@@ -2025,6 +2025,18 @@
   </si>
   <si>
     <t>InternalFun::StringToDouble(#s);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#val v=#s.top();
+#s.pop();
+#s.push(#new(std::to_string(v.floatVal())));</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#val v=#s.top();
+#s.pop();
+#s.push(v.boolVal()?#new("true"):#new("false"));</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3579,10 +3591,10 @@
   <dimension ref="A1:I320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H105" sqref="H105"/>
+      <selection pane="bottomRight" activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -4491,7 +4503,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A55" s="26"/>
       <c r="B55" s="18" t="str">
         <f t="shared" si="1"/>
@@ -4502,6 +4514,9 @@
       </c>
       <c r="D55" s="12" t="s">
         <v>291</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -4992,7 +5007,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A85" s="26"/>
       <c r="B85" s="18" t="str">
         <f t="shared" si="2"/>
@@ -5003,6 +5018,9 @@
       </c>
       <c r="D85" s="12" t="s">
         <v>291</v>
+      </c>
+      <c r="H85" s="13" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Change domain, vm to static
</commit_message>
<xml_diff>
--- a/doc/FayLang.xlsx
+++ b/doc/FayLang.xlsx
@@ -2076,12 +2076,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PTR(FayFun) fun=FayLang::Domain.findFun(#v1,#v2,true);
-this-&gt;_run(fun);</t>
-  </si>
-  <si>
-    <t>PTR(fay::FayInstance) obj = MKPTR(fay::FayInstance)(FayLang::Domain.findClass(#v1));
+    <t>PTR(fay::FayInstance) obj = MKPTR(fay::FayInstance)(#domain.findClass(#v1));
 #s.push(#val(obj));</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PTR(FayClass) clazz = #domain.useClass(#v1);
+PTR(FayFun) fun = clazz-&gt;findFun(#v2, true);
+this-&gt;_run(#s, fun);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3645,10 +3648,10 @@
   <dimension ref="A1:I321"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C305" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H321" sqref="H321"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -3958,7 +3961,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>395</v>
       </c>
@@ -3980,7 +3983,7 @@
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="13" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
@@ -8814,16 +8817,20 @@
         <v>500</v>
       </c>
       <c r="H321" s="13" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A271:A280"/>
-    <mergeCell ref="A281:A290"/>
-    <mergeCell ref="A291:A300"/>
-    <mergeCell ref="A301:A310"/>
-    <mergeCell ref="A311:A320"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="A188:A197"/>
+    <mergeCell ref="A178:A187"/>
+    <mergeCell ref="A168:A177"/>
+    <mergeCell ref="A158:A167"/>
+    <mergeCell ref="A148:A157"/>
+    <mergeCell ref="A138:A147"/>
+    <mergeCell ref="A28:A127"/>
     <mergeCell ref="A251:A260"/>
     <mergeCell ref="A261:A270"/>
     <mergeCell ref="A19:A21"/>
@@ -8835,15 +8842,11 @@
     <mergeCell ref="A231:A240"/>
     <mergeCell ref="A241:A250"/>
     <mergeCell ref="A128:A137"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A7:A13"/>
-    <mergeCell ref="A188:A197"/>
-    <mergeCell ref="A178:A187"/>
-    <mergeCell ref="A168:A177"/>
-    <mergeCell ref="A158:A167"/>
-    <mergeCell ref="A148:A157"/>
-    <mergeCell ref="A138:A147"/>
-    <mergeCell ref="A28:A127"/>
+    <mergeCell ref="A271:A280"/>
+    <mergeCell ref="A281:A290"/>
+    <mergeCell ref="A291:A300"/>
+    <mergeCell ref="A301:A310"/>
+    <mergeCell ref="A311:A320"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>